<commit_message>
Changed a lot of code here
</commit_message>
<xml_diff>
--- a/regular-expressions/Regular Expressions Project/Regular Expressions Project Answers.xlsx
+++ b/regular-expressions/Regular Expressions Project/Regular Expressions Project Answers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaydenH\Code\DATA-1040-2022\regular-expressions\Regular Expressions Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED066EA1-9408-493C-8377-6DEA45312E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4D1479-6345-40E2-9B6C-E715FE953E7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10650" xr2:uid="{B8EB5382-C987-4047-B84F-EF3493C94719}"/>
@@ -544,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972BAF2C-00C1-4D1D-B11C-36D31CA93421}">
-  <dimension ref="B1:L14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -822,7 +822,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>19</v>

</xml_diff>